<commit_message>
Resolved issue with extra row with headers in TaskResourcesTbl.
</commit_message>
<xml_diff>
--- a/production_system_intake.xlsx
+++ b/production_system_intake.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Classes\2025_01_Spring\ASU\Computation\Week03\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Classes\2025_01_Spring\ASU\Computation\Week03\Project\Dev\CAS502Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC18DDE-FC0A-41A7-8B57-58FC67BFF982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0D96B7-0646-4C0E-B352-2D1BC9D41047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" tabRatio="857" firstSheet="9" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2130" windowWidth="29040" windowHeight="15840" tabRatio="857" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessorTypeTbl" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="269">
   <si>
     <t>TaskIndex</t>
   </si>
@@ -368,54 +368,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>Quality Inspector</t>
-  </si>
-  <si>
-    <t>Mech Tech</t>
-  </si>
-  <si>
-    <t>Flotron</t>
-  </si>
-  <si>
-    <t>Panel Assmebly Stands</t>
-  </si>
-  <si>
-    <t>SV/Prop Lifting Sling</t>
-  </si>
-  <si>
-    <t>SV Lifting GS</t>
-  </si>
-  <si>
-    <t>TVAC Config GSE</t>
-  </si>
-  <si>
-    <t>Stack Lifting GSE</t>
-  </si>
-  <si>
-    <t>Dynamics Config GSE</t>
-  </si>
-  <si>
-    <t>Vacuum Chamber</t>
-  </si>
-  <si>
-    <t>Digital Multi Meter</t>
-  </si>
-  <si>
-    <t>Prop GSE</t>
-  </si>
-  <si>
-    <t>GPS Sim</t>
-  </si>
-  <si>
-    <t>Mass Prop GSE</t>
-  </si>
-  <si>
-    <t>Host Rack</t>
-  </si>
-  <si>
-    <t>Hardware Delivered from Inventory</t>
-  </si>
-  <si>
     <t>ProcessorTypeIndex</t>
   </si>
   <si>
@@ -534,45 +486,6 @@
   </si>
   <si>
     <t>TasksDesc</t>
-  </si>
-  <si>
-    <t>Egnr</t>
-  </si>
-  <si>
-    <t>Tech</t>
-  </si>
-  <si>
-    <t>MI tech</t>
-  </si>
-  <si>
-    <t>Sys01 Rack</t>
-  </si>
-  <si>
-    <t>Sys02 Rack</t>
-  </si>
-  <si>
-    <t>Sys03 Rack</t>
-  </si>
-  <si>
-    <t>Sys04 Rack</t>
-  </si>
-  <si>
-    <t>Stimulator</t>
-  </si>
-  <si>
-    <t>Sys05 Rack</t>
-  </si>
-  <si>
-    <t>Sys06 rack</t>
-  </si>
-  <si>
-    <t>Sys07 Rack (traveler)</t>
-  </si>
-  <si>
-    <t>Sys00 Rack (Workcell)</t>
-  </si>
-  <si>
-    <t>SV w/ Panels</t>
   </si>
   <si>
     <t>NResource01</t>
@@ -1358,13 +1271,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1395,31 +1308,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1450,31 +1363,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1507,43 +1420,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -2239,37 +2152,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2306,40 +2219,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>204</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2370,31 +2283,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2424,28 +2337,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,58 +2400,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="G1" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="H1" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="I1" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="J1" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="K1" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="L1" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="M1" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="N1" t="s">
-        <v>297</v>
+        <v>268</v>
       </c>
       <c r="O1" t="s">
-        <v>253</v>
+        <v>224</v>
       </c>
       <c r="P1" t="s">
-        <v>254</v>
+        <v>225</v>
       </c>
       <c r="Q1" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="R1" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2567,37 +2480,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>284</v>
+        <v>255</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="D1" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="E1" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="F1" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="G1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="H1" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="J1" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="K1" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2634,19 +2547,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2687,67 +2600,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="E1" t="s">
-        <v>266</v>
+        <v>237</v>
       </c>
       <c r="F1" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
       <c r="G1" t="s">
-        <v>265</v>
+        <v>236</v>
       </c>
       <c r="H1" t="s">
-        <v>263</v>
+        <v>234</v>
       </c>
       <c r="I1" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="J1" t="s">
-        <v>260</v>
+        <v>231</v>
       </c>
       <c r="K1" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="L1" t="s">
-        <v>268</v>
+        <v>239</v>
       </c>
       <c r="M1" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="N1" t="s">
-        <v>261</v>
+        <v>232</v>
       </c>
       <c r="O1" t="s">
-        <v>262</v>
+        <v>233</v>
       </c>
       <c r="P1" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="Q1" t="s">
-        <v>272</v>
+        <v>243</v>
       </c>
       <c r="R1" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="S1" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="T1" t="s">
-        <v>269</v>
+        <v>240</v>
       </c>
       <c r="U1" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2841,13 +2754,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3039,7 +2952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA296F8-8227-499C-B3D4-F942CBC18395}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3053,19 +2966,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="D1" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="E1" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3651,7 +3564,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -3945,10 +3858,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E098E04-19A8-4E79-81CD-069FB2C95590}">
-  <dimension ref="A1:BA30"/>
+  <dimension ref="A1:BA29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD82"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3978,257 +3891,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="U1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="V1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" t="s">
-        <v>106</v>
-      </c>
-      <c r="J1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>114</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="S1" t="s">
-        <v>115</v>
-      </c>
-      <c r="T1" t="s">
-        <v>163</v>
-      </c>
-      <c r="U1" t="s">
-        <v>116</v>
-      </c>
-      <c r="V1" t="s">
-        <v>164</v>
-      </c>
-      <c r="W1" t="s">
-        <v>165</v>
-      </c>
-      <c r="X1" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4323,34 +4147,34 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4385,22 +4209,22 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -4412,10 +4236,10 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>103</v>
@@ -4444,13 +4268,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4476,22 +4300,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>